<commit_message>
SPYlearner - first version, without EQs and optimizations like extending the last queried path
</commit_message>
<xml_diff>
--- a/data/experiments/results_peterson2_sched4_sched5.xlsx
+++ b/data/experiments/results_peterson2_sched4_sched5.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$R$59</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="46">
   <si>
     <t>Correct</t>
   </si>
@@ -146,6 +149,12 @@
   </si>
   <si>
     <t>maxDistLen:2+EQ</t>
+  </si>
+  <si>
+    <t>SPYlearner</t>
+  </si>
+  <si>
+    <t>ExtraStates:2+EQ</t>
   </si>
 </sst>
 </file>
@@ -974,10 +983,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R55"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1094,7 +1104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1147,7 +1157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1200,7 +1210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1253,7 +1263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1306,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1359,7 +1369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1412,7 +1422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1465,7 +1475,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1515,7 +1525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1565,7 +1575,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1615,7 +1625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1668,7 +1678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1721,7 +1731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1774,7 +1784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1880,7 +1890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1933,7 +1943,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2931,7 +2941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2984,7 +2994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3037,7 +3047,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -3090,7 +3100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3143,7 +3153,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3196,7 +3206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3249,7 +3259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3302,7 +3312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3355,7 +3365,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3405,7 +3415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -3455,7 +3465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3505,7 +3515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3558,7 +3568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -3611,7 +3621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -3664,7 +3674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -3717,7 +3727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
@@ -3770,7 +3780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -3823,7 +3833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -3876,7 +3886,226 @@
         <v>21</v>
       </c>
     </row>
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>50</v>
+      </c>
+      <c r="D56">
+        <v>18</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>17078</v>
+      </c>
+      <c r="G56">
+        <v>17302</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>129532</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>18.547377999999998</v>
+      </c>
+      <c r="M56" t="s">
+        <v>44</v>
+      </c>
+      <c r="N56" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56" t="s">
+        <v>20</v>
+      </c>
+      <c r="R56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>50</v>
+      </c>
+      <c r="D57">
+        <v>18</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>293439</v>
+      </c>
+      <c r="G57">
+        <v>293816</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>2495242</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>28.324876</v>
+      </c>
+      <c r="M57" t="s">
+        <v>44</v>
+      </c>
+      <c r="N57" t="s">
+        <v>45</v>
+      </c>
+      <c r="O57">
+        <v>2</v>
+      </c>
+      <c r="P57" t="s">
+        <v>20</v>
+      </c>
+      <c r="R57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>97</v>
+      </c>
+      <c r="D58">
+        <v>12</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>16498</v>
+      </c>
+      <c r="G58">
+        <v>17106</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>207606</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>35.058551999999999</v>
+      </c>
+      <c r="M58" t="s">
+        <v>44</v>
+      </c>
+      <c r="N58" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+      <c r="P58" t="s">
+        <v>20</v>
+      </c>
+      <c r="R58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>97</v>
+      </c>
+      <c r="D59">
+        <v>12</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>172412</v>
+      </c>
+      <c r="G59">
+        <v>173577</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>2297891</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>48.350580000000001</v>
+      </c>
+      <c r="M59" t="s">
+        <v>44</v>
+      </c>
+      <c r="N59" t="s">
+        <v>45</v>
+      </c>
+      <c r="O59">
+        <v>2</v>
+      </c>
+      <c r="P59" t="s">
+        <v>20</v>
+      </c>
+      <c r="R59" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:R59">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="97"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:R55">
     <sortCondition ref="C2:C55"/>
     <sortCondition ref="O2:O55"/>

</xml_diff>